<commit_message>
Upload EBA stress test tables
</commit_message>
<xml_diff>
--- a/Data_in_changes/Testing/macro_37_test.xlsx
+++ b/Data_in_changes/Testing/macro_37_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BuDA_2.0_Oct2017\User Supplied Macro\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Projects\EBA\Data_in_changes\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -75,7 +75,7 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>Finland</t>
+    <t>France</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +564,7 @@
         <v>-0.100000000000001</v>
       </c>
       <c r="E18">
-        <v>1.61160354552778</v>
+        <v>1.7</v>
       </c>
       <c r="F18">
         <v>0.68500000000000005</v>
@@ -593,7 +593,7 @@
         <v>-9.9999999999999603E-2</v>
       </c>
       <c r="E19">
-        <v>-0.23591860808022599</v>
+        <v>0.6</v>
       </c>
       <c r="F19">
         <v>0.96499999999999997</v>
@@ -623,7 +623,7 @@
         <v>-0.1</v>
       </c>
       <c r="E20">
-        <v>-0.15757337010046499</v>
+        <v>-0.1</v>
       </c>
       <c r="F20">
         <v>0.82140000000000002</v>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>-0.58479532163741499</v>
+        <v>0.6</v>
       </c>
       <c r="F21">
         <v>0.74739999999999995</v>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0.89905208638718603</v>
+        <v>1.2</v>
       </c>
       <c r="F22">
         <v>0.78500000000000003</v>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="E18">
         <f>'Test 1'!E18</f>
-        <v>1.61160354552778</v>
+        <v>1.7</v>
       </c>
       <c r="F18">
         <f>'Test 1'!F18</f>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="E19">
         <f>'Test 1'!E19</f>
-        <v>-0.23591860808022599</v>
+        <v>0.6</v>
       </c>
       <c r="F19">
         <f>'Test 1'!F19</f>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="E20">
         <f>'Test 1'!E20</f>
-        <v>-0.15757337010046499</v>
+        <v>-0.1</v>
       </c>
       <c r="F20">
         <f>'Test 1'!F20</f>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="E21">
         <f>'Test 1'!E21</f>
-        <v>-0.58479532163741499</v>
+        <v>0.6</v>
       </c>
       <c r="F21">
         <f>'Test 1'!F21</f>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="E22">
         <f>'Test 1'!E22</f>
-        <v>0.89905208638718603</v>
+        <v>1.2</v>
       </c>
       <c r="F22">
         <f>'Test 1'!F22</f>

</xml_diff>